<commit_message>
add definition and parent in OBI
</commit_message>
<xml_diff>
--- a/docs/developer/anatomy/OBIanatomy.update.xlsx
+++ b/docs/developer/anatomy/OBIanatomy.update.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25260" windowHeight="4575" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>peritoneum</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -264,22 +264,84 @@
     <t>http://purl.obolibrary.org/obo/OBI_0302745</t>
   </si>
   <si>
-    <t>notes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>liver</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0302743</t>
+  </si>
+  <si>
+    <t>Parent in OBI</t>
+  </si>
+  <si>
+    <t>http://www.ifomis.org/bfo/1.1/snap#MaterialEntity</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Anatomical structure that is part of a multicellular organism and is at the gross anatomical level, e.g. above the level of a cell.  Included are portions of organism substances such as blood, multi-cell-part structures such as axon tracts, acellular anatomical structures such as hair, and organism subdivisions such as head. Excluded is the whole organism and more granular parts of the organism, such as atoms, molecules, macromolecular complexes and cells.</t>
+  </si>
+  <si>
+    <t>The brain is the center of the nervous system in all vertebrate, and most invertebrate, animals.[1] Some primitive animals such as jellyfish and starfish have a decentralized nervous system without a brain, while sponges lack any nervous system at all. In vertebrates, the brain is located in the head, protected by the skull and close to the primary sensory apparatus of vision, hearing, balance, taste, and smell[WP].</t>
+  </si>
+  <si>
+    <t>Oval or bean shaped bodies (1 - 30 mm in diameter) located along the lymphatic system. Lymph nodes are garrisons of B, T, and other immune cells. Lymph nodes are found all through the body, and act as filters or traps for foreign particles. They contain white blood cells that use oxygen to process. Thus they are important in the proper functioning of the immune system. The lymph node is surrounded by a fibrous capsule, and inside the lymph node the fibrous capsule extends to form trabeculae. The substance of the lymph node is divided into the outer cortex and the inner medulla surrounded by the former all around except for at the hilum, where the medulla comes in direct contact with the surface. Thin reticular fibers, elastin and reticular fibers form a supporting meshwork called reticular network (RN) inside the node, within which the white blood cells (WBCs), most prominently, lymphocytes are tightly packed as follicles in the cortex. Elsewhere, there are only occasional WBCs. The RN provides not just the structural support, but also provide surface for adhesion of the dendritic cells, macrophages and lymphocytes. It allows for exchange of material with blood through the high endothelial venules and provides the growth and regulatory factors necessary for activation and maturation of immune cells[WP].</t>
+  </si>
+  <si>
+    <t>script worked</t>
+  </si>
+  <si>
+    <t>Circulating body substance which consists of blood plasma and hemoglobin-carrying red blood cells. Excludes blood analogues (see UBERON:0000179 haemolymphatic fluid).</t>
+  </si>
+  <si>
+    <t>Organ found in virtually all vertebrate animals with important roles in regard to red blood cells and the immune system.[1] In humans, it is located in the left upper quadrant of the abdomen. It removes old red blood cells and holds a reserve in case of hemorrhagic shock, especially in animals like horses (not in humans), while recycling iron.[2] It synthesizes antibodies in its white pulp and removes, from blood and lymph node circulation, antibody-coated bacteria along with antibody-coated blood cells.</t>
+  </si>
+  <si>
+    <t>Nucleus of brain which is an elongated crescent-shaped mass lying parallel and adjacent to the lateral ventricle throughout its extent.</t>
+  </si>
+  <si>
+    <t>The dermis is a layer of skin between the epidermis (with which it makes up the skin) and subcutaneous tissues, and is composed of two layers, the papillary and reticular dermis[WP].</t>
+  </si>
+  <si>
+    <t>First portion of the digestive tract[WP]. The portion of the digestive that develops from the stomodeum</t>
+  </si>
+  <si>
+    <t>Any of the tubular branching vessels that carry blood from the capillaries toward the heart.</t>
+  </si>
+  <si>
+    <t>Dense irregular connective tissue, which predominantly consists of adipocytes. Fat is stored in adipose tissue.</t>
+  </si>
+  <si>
+    <t>An exocrine gland which secretes bile and functions in metabolism of protein and carbohydrate and fat, synthesizes substances involved in the clotting of the blood, synthesizes vitamin A, detoxifies poisonous substances, stores glycogen, and breaks down worn-out erythrocytes[GO].</t>
+  </si>
+  <si>
+    <t>A serous membrane that forms the lining of the abdominal cavity or the coelom — it covers most of the intra-abdominal (or coelomic) organs — in higher vertebrates and some invertebrates (annelids, for instance). It is composed of a layer of mesothelium supported by a thin layer of connective tissue. The peritoneum both supports the abdominal organs and serves as a conduit for their blood and lymph vessels and nerves[WP]. The smooth transparent serous membrane that lines the cavity of the abdomen of a mammal and is folded inward over the abdominal and pelvic viscera[BTO]. The endothelial lining of the ABDOMINAL CAVITY. The parietal peritoneum covers the inside of the ABDOMINAL WALL and the visceral peritoneum covers the bowel, the MESENTERY, and certain of the organs. The portion that covers the bowel becomes the serosal layer of the bowel wall[GAID].</t>
+  </si>
+  <si>
+    <t>Lowermost layer of the integumentary system in vertebrates. Types of cells that are found in the hypodermis are fibroblasts, adipose cells, and macrophages. It is derived from the mesoderm, but unlike the dermis, it is not derived from the dermatome region of the mesoderm. The hypodermis is used mainly for fat storage[WP]. A layer separating the inner face of the dermis from the subjacent muscle cells. It is covered on both sides by a basement membrane. It contains pigment cells[FMA].</t>
+  </si>
+  <si>
+    <t>A mucosa that is part of a nasopharynx [Obol].</t>
+  </si>
+  <si>
+    <t>A mucosa that is part of a oropharynx [Obol].</t>
+  </si>
+  <si>
+    <t>Tissue which consists of skeletal muscle fibers surrounded by endomysium. Examples: Skeletal muscle tissue of biceps, Skeletal muscle tissue of diaphragm[FMA]. Striated muscle tissue under control of the somatic nervous system. It is one of three major muscle types, the others being cardiac and smooth muscle. As its name suggests, most skeletal muscle is attached to bones by bundles of collagen fibers known as tendons. Skeletal muscle is made up of individual components known as muscle fibers. These fibers are formed from the fusion of developmental myoblasts. The myofibers are long, cylindrical, multinucleated cells composed of actin and myosin myofibrils repeated as a sarcomere, the basic functional unit of the cell and responsible for skeletal muscle's striated appearance and forming the basic machinery necessary for muscle contraction. The term muscle refers to multiple bundles of muscle fibers held together by connective tissue[WP].</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CARO_0000055</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CARO_0000043</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -291,6 +353,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -311,10 +379,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -322,8 +394,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -650,22 +729,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -678,11 +758,14 @@
       <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="26">
+      <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -692,11 +775,17 @@
       <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="26">
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -709,8 +798,14 @@
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="26">
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -723,8 +818,14 @@
       <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="26">
+      <c r="E4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -737,8 +838,14 @@
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="26">
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -751,8 +858,14 @@
       <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="26">
+      <c r="E6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -765,8 +878,14 @@
       <c r="D7" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="52">
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="51">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -779,8 +898,14 @@
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="26">
+      <c r="E8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -793,8 +918,14 @@
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="26">
+      <c r="E9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -807,8 +938,14 @@
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="26">
+      <c r="E10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -821,8 +958,14 @@
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="26">
+      <c r="E11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -835,22 +978,34 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="26">
+      <c r="E12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5">
       <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="26">
+      <c r="E13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,8 +1018,14 @@
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="26">
+      <c r="E14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -877,8 +1038,14 @@
       <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="26">
+      <c r="E15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25.5">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -891,8 +1058,14 @@
       <c r="D16" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="26">
+      <c r="E16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -905,8 +1078,14 @@
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="26">
+      <c r="E17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -919,9 +1098,20 @@
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="E18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" location="CARO_0000004" display="http://purl.org/obo/owl/CARO#CARO_0000004"/>
+    <hyperlink ref="E3" r:id="rId2" location="CARO_0001008" display="http://purl.org/obo/owl/CARO#CARO_0001008"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>